<commit_message>
remove duplicate and complainted url in report_handsha.py
</commit_message>
<xml_diff>
--- a/data_saved/exact_country_log.xlsx
+++ b/data_saved/exact_country_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2317,13 +2317,15 @@
           <t>https://ninjasuplementos.blogspot.com/?gclid=EAIaIQobChMIyovU48m29gIVCFdgCh1n3AoVEAAYASAAEgI4OPD_BwE</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="A31" t="n">
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2351,7 +2353,7 @@
         </is>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44628.87856002746</v>
+        <v>44628.87856002315</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2378,7 +2380,2464 @@
           <t>https://vwv-kukoiin.net/?id=dip</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.82 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>44628.94931310185</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj-i43t4Lb2AhWEQ2AKHTPMBnsYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1Hd5V6M9ELJ6ajD_4BjrWVmr-Iiw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=X2wnYrvFHcaUr7wP4rqX6Ao&amp;iflsig=AHkkrS4AAAAAYid6b65YcCTDv1k_K2inl_UlqJUQM3Nm&amp;ved=0ahUKEwj78I_r4Lb2AhVGyosBHWLdBa0Q4dUDCAg&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWARg0hdoAHAAeAKAAXOIAZkDkgEDMS4zmAEAoAEB&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign in</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>We are much more than a wallet</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.27 Safari/537.36 Edg/96.0.1054.8</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>44628.95049100694</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwigr7yd4bb2AhWJXWAKHc2YBrwYABADGgJ0bQ&amp;ae=2&amp;sig=AOD64_02FCYE4jB7jHyHNMxrzavL5osWsg&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=xGwnYoe_EeHcmAXJ8qDQBw&amp;iflsig=AHkkrS4AAAAAYid61BTBnDRGmT9eG1QHFaicewrzSrBh&amp;ved=0ahUKEwiHsZib4bb2AhVhLqYKHUk5CHoQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYOUXaABwAHgBgAFaiAHbApIBATSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign in</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>We are much more than a wallet</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; EML-AL00 Build/HUAWEIEML-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>44628.95136407408</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiK5dDB4bb2AhUGt5YKHclUC6AYABAAGgJ0bA&amp;sig=AOD64_2pzgsaoMIPfEz_MDqqyfGsxie2nA&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=EG0nYsyGMMaWr7wPkuqniA8&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUANYBWDbF2gAcAB4AoABYogB7QKSAQE0mAEAoAEBsAEA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Kucoin lets you buy, sell, and store. Official Website. kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome.</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.55 Safari/537.36 Edg/96.0.1054.43</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>kok-IN</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>kok-IN</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>44628.95220553241</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjR4Pnj4bb2AhXKQ2AKHdWYDLcYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_3BrdgaSbo1UVPJ_Txuj-WWQDLxsA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=WG0nYtmjEu2umAXIoKh4&amp;iflsig=AHkkrS4AAAAAYid7aDVFE4qaJVLw4hdfJy2Wb1qDumcK&amp;ved=0ahUKEwjZr-Lh4bb2AhVtF6YKHUgQCg8Q4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYN0XaABwAHgCgAFqiAGVA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (3794MB; 1440x2417; 554x555; 423x710; LGE LGLS992; 7.0) AppleWebKit/537.36 (KHTML, like Gecko) ROBLOX Android App 2.389.310791 Phone Hybrid() GooglePlayStore</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>44628.95272871528</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiOj-v54bb2AhVGrpYKHT9rCBYYABAAGgJ0bA&amp;sig=AOD64_2YRm5T1lBGfnMA4UU-i4u_gEQEew&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=hm0nYtKeCIf10ASYhangCA&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUARYB2DYF2gAcAB4AYABrgKIAYoJkgEFMi0zLjGYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.102 Safari/537.36 Edg/98.0.1108.56</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>gu-IN</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>gu-IN</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>44628.95637572917</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjq65GQ47b2AhW43EwCHdOwDnMYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_2KYpH2u-oIYErVTm2cApu5Z36QbQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=wW4nYpaUIszemAWB972wCQ&amp;iflsig=AHkkrS4AAAAAYid80dttWzpP-JCkVogR3UKQ00SSvUjE&amp;ved=0ahUKEwjW-IOO47b2AhVML6YKHYF7D5YQ4dUDCAg&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEUABYBGDXF2gAcAB4A4ABcogBpwOSAQMxLjOYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:91.0) Gecko/20100101 Firefox/91.0</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>44628.95689670139</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjoxNGl47b2AhVCTmAKHdfHCPMYABAAGgJ0bQ&amp;sig=AOD64_0evhCAzOiNCKWTP9nMxt8QIPosUA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=7m4nYsKXFbKRr7wP0cc6&amp;iflsig=AHkkrS4AAAAAYid8_szYz6E4jzKPqID96DGq7ZgJRHsD&amp;ved=0ahUKEwjCxrGj47b2AhWyyIsBHdGjDgAQ4dUDCAc&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWARg0BdoAHAAeAGAAXOIAZUDkgEDMS4zmAEAoAEB&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 11; Pixel 5) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/84.0.4147.111 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>ta-IN</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>ta-IN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>44628.95808744213</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjk48PW47b2AhWbwhYFHYAdC_gYABACGgJ0bA&amp;ae=2&amp;sig=AOD64_1L1mMXONDwiOzwG9V3HH3bX83Y2g&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=VW8nYrWhF5XemAWlx7vYBg&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgMYNgXaABwAHgBgAFbiAHbApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>https://shoptimex.blogspot.com/?gclid=EAIaIQobChMI5OPD1uO29gIVm8IWBR2AHQv4EAAYASAAEgKr-vD_BwE&amp;m=1</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/92.0.4476.0 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>ta-IN</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>ta-IN</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>44628.95860773148</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiqs-Hr47b2AhVVQWAKHe2JAlEYABABGgJ0bQ&amp;ae=2&amp;sig=AOD64_2mm0t8JIts8v2aHLfodyVx0dzn4g&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=gm8nYueGApCFr7wPgOO5oAU&amp;iflsig=AHkkrS4AAAAAYid9kufSdZQ1gypA0aXHR_2gB1YXOywR&amp;ved=0ahUKEwjnz-fp47b2AhWQwosBHYBxDlQQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYNEXaABwAHgCgAFjiAH4ApIBATSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/99.0.7113.93 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>44628.95977946759</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi6uqOc5Lb2AhXL1pYKHdZVBtIYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_3wUuiOa59s7MSR837_-ck_q37hIA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=528nYpijLcWzmAWA1bHABQ&amp;iflsig=AHkkrS4AAAAAYid990LE5D0QyK-PQB-5p_S0cFp-UkRk&amp;ved=0ahUKEwjYsqea5Lb2AhXFGaYKHYBqDFgQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYNoXaABwAHgAgAFriAGPA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:98.0) Gecko/20100101 Firefox/98.0</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>44628.96030321759</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjA4NGx5Lb2AhVBdGAKHUWVAW4YABAAGgJ0bQ&amp;sig=AOD64_1A1tuD0mt1Cz_QyXcMpuJ04rMgDA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=FHAnYoPoIZTdmAWY546ICA&amp;iflsig=AHkkrS4AAAAAYid-JHg6n-OLXOV_GqGMIRrgjMe-fgCz&amp;ved=0ahUKEwiDwtav5Lb2AhWULqYKHZizA4EQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNwXaABwAHgBgAFuiAGfA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 14_7 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) CriOS/92.0.4515.90 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>kn-IN</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>kn-IN</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>44628.96114679398</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi1i8zU5Lb2AhULEGAKHWcTBAUYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_211p9tTvt-RIkFRppg2xHt8d1Vxw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=XXAnYvCdMYHemAXs-ZOoBA&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUARYB2DaF2gAcAB4AYABdIgBmQOSAQMyLjKYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/99.0.4844.51 Safari/537.36 Edg/99.0.1150.30</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>44628.96265842592</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjWo7uS5bb2AhXYXWAKHbGVDlsYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_2XZHgS-Av3XX9EAWzvp_86obycgw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=3nAnYvDVOIWN-Aa-o4D4Cw&amp;iflsig=AHkkrS4AAAAAYid-7sLkWghY6aw-ryKWCHA2_ZjDFhAh&amp;ved=0ahUKEwjwvJaQ5bb2AhWFBt4KHb4RAL8Q4dUDCAg&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWAVg0BdoAHAAeAGAAZoBiAG3BJIBAzAuNJgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign In</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Log in is a secure currency exchange that makes it easier to buy。btenha sua primeira cripto hoje!</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 11; M2102K1G) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/91.0.4472.101 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>44628.96318394676</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiUn7Oo5bb2AhWR0pYKHVeADWsYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_2c54IScWXpP3WQ1Hf4SPd72SdxXw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=DHEnYouvLdHEmAWN7YqYAg&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUANYBmDRF2gAcAB4AoABb4gBgQOSAQMzLjGYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.102 Safari/537.36 Edg/98.0.1108.56</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>44628.96402643518</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjftpXL5bb2AhWTQ2AKHYGXBbgYABABGgJ0bQ&amp;ae=2&amp;sig=AOD64_0CjkzpcAJOktsZmeOHgtS2XHQ1nQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=VXEnYqf8OpOC0wSVlKrgDg&amp;iflsig=AHkkrS4AAAAAYid_ZWT9XHf8PUvRulTVkXWgJ_byvGdS&amp;ved=0ahUKEwjn-vfI5bb2AhUTwZQKHRWKCuwQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgIYNkXaABwAHgBgAGLAYgB-QOSAQMwLjSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; ALP-AL00 Build/HUAWEIALP-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>44628.96453200231</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjz7org5bb2AhUPeSoKHcqoDz4YABABGgJ0bQ&amp;sig=AOD64_1q3YKih5HPm8dZal7WuO0gxBYHIw&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=gnEnYqKeH_qEr7wPn-aq-AQ&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNAXaABwAHgBgAFiiAH9ApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>https://shoptimex.blogspot.com/?gclid=EAIaIQobChMI8-6K4OW29gIVD3kqCh3KqA8-EAAYASAAEgLIc_D_BwE&amp;m=1</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/92.0.4476.0 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G48" s="2" t="n">
+        <v>44628.9650574074</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjf6dT15bb2AhXOXWAKHbc0DO0YABACGgJ0bQ&amp;ae=2&amp;sig=AOD64_1npWvh4WDuG8ii-UnAvG9d0mIKlg&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=r3EnYqOlJ8ndmAWFobyYBg&amp;iflsig=AHkkrS4AAAAAYid_v5RI9pgcvtykHvgssqvHGlE7pMMp&amp;ved=0ahUKEwjjuNnz5bb2AhXJLqYKHYUQD2MQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgLYOAXaABwAHgAgAGFAYgB4QOSAQMxLjOYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:96.0) Gecko/20100101 Firefox/96.0</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>44628.96560335648</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjl1J2M5rb2AhUYVGAKHVcxAZcYABAAGgJ0bQ&amp;sig=AOD64_1YCPfaV8r4fil_nT-ny8TPshZtew&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=3nEnYrLJOeiLr7wPp96jsAs&amp;iflsig=AHkkrS4AAAAAYid_7mEzF6p9m4N2QzPgq4RyoCr3Ai0d&amp;ved=0ahUKEwiysKCK5rb2AhXoxYsBHSfvCLYQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgIYM8XaABwAHgBgAFkiAH4ApIBAzIuMpgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>KuCoin - Sign Up Platform - Home Welcome Exchange Trade</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>kucoin: Log in is a secure currency exchange that makes it easier to buy. Welcome. Kucoin lets you buy, sell, and store. Official Website.</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; zh-cn; BRQ-AN00 Build/HUAWEIBRQ-AN00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Chrome/77.0.3865.120 MQQBrowser/11.9 Mobile Safari/537.36 COVC/045717</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>44628.96644335648</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjlgteu5rb2AhUSt5YKHfc3DtwYABAAGgJ0bA&amp;sig=AOD64_0y_8k_VIzR-I5Aw8O3ozZ20BRtxw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=J3InYqnGEsmHr7wPyPWakAc&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUANYB2DeF2gAcAB4AYABZIgBhQOSAQMyLjKYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign In</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Log in is a secure currency exchange that makes it easier to buy。btenha sua primeira cripto hoje!</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/92.0.4476.0 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>44628.96730359954</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj0kaTS5rb2AhXFUGAKHa4MA2IYABACGgJ0bQ&amp;ae=2&amp;sig=AOD64_1p9IZtzdyoQkzyqM3BVmHjY0maVw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=cXInYu2SOIeJmAWZtLrgCg&amp;iflsig=AHkkrS4AAAAAYieAgWtZwo7BrOzyjWVu8K-aDZgTzNYR&amp;ved=0ahUKEwitj6vQ5rb2AhWHBKYKHRmaDqwQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYOAXaABwAHgBgAFsiAGWA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign in</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>We are much more than a wallet</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.93 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>44628.97035321759</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwie26DP57b2AhVDdmAKHR9kCIcYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_0wYTohA07chbuXSgX-LiSP5GAkPw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=dnMnYuOBGbTcmAWK6JH4Cg&amp;iflsig=AHkkrS4AAAAAYieBhgZvVTRiRJ-pFco5upOeccbeBm5f&amp;ved=0ahUKEwjjlMbM57b2AhU0LqYKHQp0BK8Q4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYNcXaABwAHgCgAF6iAHSA5IBAzAuNJgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign in - Platform Secure</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>We are much more than a wallet</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 10_3_1 like Mac OS X) AppleWebKit/603.1.30 (KHTML, like Gecko) Version/10.0 Mobile/14E304 Safari/602.1</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G53" s="2" t="n">
+        <v>44628.9708962963</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj1r83k57b2AhUE2JYKHct0CeUYABAAGgJ0bA&amp;sig=AOD64_0dTsE8egEl8nLrZYVuaZStUEfFfw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=pHMnYvPpNOOTr7wP5qm1qAo&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNcXaABwAHgBgAFWiAHPApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Log In</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>https://lojamundofisio.blogspot.com/?gclid=EAIaIQobChMI9a_N5Oe29gIVBNiWCh3LdAnlEAAYASAAEgIjzfD_BwE&amp;m=1</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:91.0) Gecko/20100101 Firefox/91.0 Waterfox/91.6.0</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G54" s="2" t="n">
+        <v>44628.97330297454</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi5hpzJ6Lb2AhVKQWAKHRi3AnkYABABGgJ0bQ&amp;sig=AOD64_3xIVIOrZRdQqEuX3k_UkOURMc1xQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=d3QnYrqREeOGr7wPh_mTuAk&amp;iflsig=AHkkrS4AAAAAYieCh4TurUIcUL0mHs5iRPY78lsL3S9B&amp;ved=0ahUKEwj6qITH6Lb2AhVjw4sBHYf8BJcQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYNgXaABwAHgBgAGTAYgBqASSAQMwLjSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up - Exchange KuCoin</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Exchange KuCoin。KuCoin is a secure exchange, a simple and secure way to buy, sell and store。</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.102 Safari/537.36 Edg/98.0.1108.62</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>gu-IN</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>gu-IN</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>44628.97449357639</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjQpsn66Lb2AhXCqZYKHY5JCGEYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_1WzntXz4fFMXalrrKaYrpKOqkLJg&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=3nQnYrWgN4OVr7wP4t-Q-As&amp;iflsig=AHkkrS4AAAAAYieC7ofN-mlDc0O8RqfDu9VaoQFHvzJV&amp;ved=0ahUKEwi1h7n46Lb2AhWDyosBHeIvBL8Q4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYN8XaABwAHgCgAFfiAHsApIBATSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in - Trading Deposit Official Site</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Kucoin the most trusted and secure exchange, Trade simple with maximum security. Kukoin Deposit Official Site。</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.18 Safari/537.36 Edg/96.0.1054.5</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>44628.97501377315</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjUxP-P6bb2AhXQ2EwCHew1AAcYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_2EqnX2moqDXtZSjDci7PffFlX5zA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=C3UnYoP1N9yVr7wP-IiJoAY&amp;iflsig=AHkkrS4AAAAAYieDG5JWYyOxZNrtLG5gaHvbegdUBiu9&amp;ved=0ahUKEwjDpvSN6bb2AhXcyosBHXhEAmQQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNQXaABwAHgCgAFyiAG0A5IBAzAuNJgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Security Platform Sign In, Join Us</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 11; moto g(50) Build/RRFS31.Q1-59-76-2; wv) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Chrome/92.0.4515.159 Mobile Safari/537.36 EdgW/1.0</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>44628.97588094907</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjZgp6z6bb2AhVKdmAKHU_6ARUYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_2aO2N4Glz3h98z82RCoxW8RJlbgQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=VXUnYoiiMbC1mAXroo7gDQ&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNUXaABwAHgCgAFaiAHiApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Log In</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>https://lojamundofisio.blogspot.com/?gclid=EAIaIQobChMI2YKes-m29gIVSnZgCh1P-gEVEAAYASAAEgIIL_D_BwE&amp;m=1</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.93 Safari/537.36 Edg/96.0.1054.53</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>44628.97652438658</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjW2vXN6bb2AhUIWmAKHaK5Aq0YABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1AxFYyr-Q9BBulZSrWmWpL11r-lg&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=i3UnYpDSA4j90ASygrXgDQ&amp;iflsig=AHkkrS4AAAAAYieDm0Yf_7ybwXUQLgxAYkn9FEroV7kZ&amp;ved=0ahUKEwjQw8TK6bb2AhWIPpQKHTJBDdwQ4dUDCAg&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWAVg0RdoAHAAeAKAAdoEiAHREpIBAzUtNJgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>KuCoin Home - Sign in</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>We are much more than a wallet</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; zh-cn; BRQ-AN00 Build/HUAWEIBRQ-AN00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Chrome/77.0.3865.120 MQQBrowser/11.9 Mobile Safari/537.36 COVC/045717</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>44628.97704159722</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjm_bXj6bb2AhUNPmAKHagaCqEYABACGgJ0bQ&amp;sig=AOD64_1I0KQAsmAenvBn7v6d7NXWHxg2Ag&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=u3UnYvzABbXCmAX6iYPICg&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gLYNEXaABwAHgCgAF_iAHkA5IBAzAuNJgBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Log In</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>https://lojamundofisio.blogspot.com/?gclid=EAIaIQobChMI5v214-m29gIVDT5gCh2oGgqhEAAYASAAEgLVUfD_BwE&amp;m=1</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/99.0.4844.45 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>44628.97760444444</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiZnuD66bb2AhWKQ2AKHeWEB-oYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_0gIPQ_zlarH7xZfb10caE88auzCA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=63UnYrvVO7GXr7wPl76t2Aw&amp;iflsig=AHkkrS4AAAAAYieD_CdparYVGB5LSZuuEN1Ffl1-Z9iu&amp;ved=0ahUKEwj79t_46bb2AhWxy4sBHRdfC8sQ4dUDCAg&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWARg1RdoAHAAeAGAAd4BiAHVBpIBBTAuMS4zmAEAoAEB&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Kucoin - Sign Up Access - Welcome To KuCoin Buy Sell</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in is a secure currency exchange that makes it easier to buy, sell, and store。Kucoin is a secure exchange。</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.35 Safari/537.36 Edg/96.0.1054.13</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>44628.97813762732</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiJ2JyQ6rb2AhWDJGAKHYpqCNkYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_0NMZMCjXY0eRPasfjsD09mz7rE7g&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=GHYnYvLcGcKImAXitpPgCA&amp;iflsig=AHkkrS4AAAAAYieEKJqaCcU2LZrFFijbkzQvTVnaNxl_&amp;ved=0ahUKEwjyyPiN6rb2AhVCBKYKHWLbBIwQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgLYNwXaABwAHgAgAFviAGDA5IBAzMuMZgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Kucoin - Kucoin Sign Up</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Exchange KuCoin。KuCoin is a secure exchange, a simple and secure way to buy, sell and store。</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>https://wvwkucolnsv.com/ucenter.txt</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/15.2 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>te-IN</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>te-IN</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>44628.97947616898</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwij4N7H6rb2AhVQPmAKHYDgBDcYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1SPdVfV0iDI77A4QwBoHiKRXJMig&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=jXYnYoqoG4q2mAX8mazQBA&amp;iflsig=AHkkrS4AAAAAYieEnfFHWQYzQiWHUdFSVD2iF5pbCpk4&amp;ved=0ahUKEwjKot_F6rb2AhUKG6YKHfwMC0oQ4dUDCAc&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWAVgzBdoAHAAeAKAAXOIAaoDkgEDMS4zmAEAoAEB&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Kucoin - Sign Up Access - Welcome To KuCoin Buy Sell</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in is a secure currency exchange that makes it easier to buy, sell, and store。Kucoin is a secure exchange。</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; CLT-AL00 Build/HUAWEICLT-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>44628.98219956019</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjwvN-367b2AhXLwRYFHTFvDNIYABAAGgJ0bA&amp;sig=AOD64_3rT1qDFeNf1abTbVKALeccD_gtNg&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=eHcnYvHzIcremAWfzbj4Aw&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUANYBmDOF2gAcAB4AYABYogB-gKSAQE0mAEAoAEBsAEA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Kucoin - Sign Up Access - Welcome To KuCoin Buy Sell</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in is a secure currency exchange that makes it easier to buy, sell, and store。Kucoin is a secure exchange。</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>kucoin login</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.102 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>44628.98272454861</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjeu73N67b2AhWXdmAKHZ1JA2EYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_0cnsrGQD2XvLN9bgs8dzTwt1raYw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+login&amp;source=hp&amp;ei=pXcnYoiJOr3fmAWgx5iwCw&amp;iflsig=AHkkrS4AAAAAYieFtW7_HtdHzNbfXDAhclNUv7YOpRRQ&amp;ved=0ahUKEwjI77_L67b2AhW9L6YKHaAjBrYQ4dUDCAg&amp;uact=5&amp;oq=kucoin+login&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeUABYB2DVF2gAcAB4AoABbogBkAOSAQMxLjOYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Ku-Coin: Log in Wallet - Ku-Coin Exchange Trading</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Buy and Sell Platform. Assets Markets Exchange。Conte com Nossa Equipe para o Projeto de Decoração de Seu Espaço. Peça Já Seu Orçamento。</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>https://vvv-kvcoln.site/ucenter/signin?f4a8a71f-3d65-4e58-92d0-11dfb12c1a9c801a368e-5b9a-41e0-862b-e7989539175a</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; in-id; SM-M205G Build/QP1A.190711.020) AppleWebKit/533.1 (KHTML, like Gecko) Mobile Safari/533.1</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>44628.98324417824</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjd3Irj67b2AhUt3EwCHRkCBkUYABAAGgJ0bQ&amp;sig=AOD64_23JOsVy1A7b9L6i2AxKkNIQZRCGQ&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=03cnYqzGGaqImAXkv6e4DA&amp;oq=kucoin&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQ6CAgAEIAEELEDUARYB2DNF2gAcAB4AoABbIgBigOSAQMzLjGYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Kucoin - Sign Up Access - Welcome To KuCoin Buy Sell</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in is a secure currency exchange that makes it easier to buy, sell, and store。Kucoin is a secure exchange。</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>kucoin login</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/15.1 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>44628.9837629051</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiG07j467b2AhVJVGAKHbGxBBgYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1twf1ULxRRLoTNo-cQcFoWRsMPBA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+login&amp;source=hp&amp;ei=AHgnYveCAuOGr7wPh_mTuAk&amp;iflsig=AHkkrS4AAAAAYieGEGjvWgOkmUbmNRfOUq3fAQVHAx9h&amp;ved=0ahUKEwj3grr267b2AhVjw4sBHYf8BJcQ4dUDCAc&amp;uact=5&amp;oq=kucoin+login&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeMgQIABAeOgYIABAKEB5QAFgJYNsXaABwAHgAgAFjiAH0ApIBATSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Ku-Coin: Log in Wallet - Ku-Coin Exchange Trading</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Buy and Sell Platform. Assets Markets Exchange。Conte com Nossa Equipe para o Projeto de Decoração de Seu Espaço. Peça Já Seu Orçamento。</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>https://vvv-kvcoln.site/ucenter/signin?bbffa392-c0dc-43ab-8eee-298c142294d15cf00ac5-6e11-4f84-a063-b900c9297e3d</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>kucoin login</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 11; SM-M127N) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Chrome/80.0.3987.119 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>te-IN</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>te-IN</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>44628.98494380787</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiO0vio7Lb2AhVXdmAKHVomAuEYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_0uYLpcLi7TTOezhSvOkOdiok_UWw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+login&amp;source=hp&amp;ei=ZXgnYv2TN5T90ATco4a4Cw&amp;oq=kucoin+login&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIECAAQHjIECAAQHjIECAAQHjIECAAQHjIECAAQHjIECAAQHjIECAAQHlADWApgzhdoAHAAeAKAAVuIAeUCkgEBNJgBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Ku-Coin: Log in Wallet - Ku-Coin Exchange Trading</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Buy and Sell Platform. Assets Markets Exchange。Conte com Nossa Equipe para o Projeto de Decoração de Seu Espaço. Peça Já Seu Orçamento。</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>https://vivadecora1.blogspot.com/2022/03/viva-decora-ideias-para-decoracao-e.html?m=1</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 11; M2103K19PG) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/91.0.4472.101 Mobile Safari/537.3</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>44628.98583116898</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi8-P7M7Lb2AhVQxJYKHSN6CesYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_07xLLTL3Xv9NPadbqR9n9YmQmyAw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=r3gnYtuzMaqImAXkv6e4DA&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gLYNEXaABwAHgBgAGbAogB5giSAQMyLTSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Ku-Coin: Log in Wallet - Ku-Coin Exchange Trading</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Buy and Sell Platform. Assets Markets Exchange。Conte com Nossa Equipe para o Projeto de Decoração de Seu Espaço. Peça Já Seu Orçamento。</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>https://vivadecora1.blogspot.com/2022/03/viva-decora-ideias-para-decoracao-e.html?m=1</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>kucoin</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:96.0) Gecko/20100101 Firefox/96.0</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G69" s="2" t="n">
+        <v>44628.98700841435</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjH-YH-7Lb2AhUUdmAKHaMeBBIYABAAGgJ0bQ&amp;sig=AOD64_1mzU3niPNT4McB17AJeAs3SPEJ6g&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin&amp;source=hp&amp;ei=GHknYqWVDtmVr7wPxZC3gA8&amp;iflsig=AHkkrS4AAAAAYieHKMyke0akR-Isyq2AWyR0NSfGn0bV&amp;ved=0ahUKEwilgYj87Lb2AhXZyosBHUXIDfAQ4dUDCAc&amp;uact=5&amp;oq=kucoin&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEOggIABCABBCxA1AAWARgxxdoAHAAeAKAAXmIAcYDkgEDMS4zmAEAoAEB&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Kucoin - Sign Up Access - Welcome To KuCoin Buy Sell</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>KuCoin: Log in is a secure currency exchange that makes it easier to buy, sell, and store。Kucoin is a secure exchange。</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>https://wab.signin-assets.com/?c=LEKINHO</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/92.0.4476.0 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>pa-IN</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>pa-IN</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>44628.98785109954</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwie_-Gg7bb2AhUSdmAKHdi4DkwYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1Pd7J2FHiGp2RbUHzHIf2FO4KgEw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=YHknYryBBqOTr7wP39y6qAQ&amp;iflsig=AHkkrS4AAAAAYieHcM158pgwGYSckNR4n1qzoJPGlTlG&amp;ved=0ahUKEwi8saqe7bb2AhWjyYsBHV-uDkUQ4dUDCAg&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNkXaABwAHgBgAGLAYgB8wOSAQMwLjSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Ku-Coin: Log in Wallet - Ku-Coin Exchange Trading</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Buy and Sell Platform. Assets Markets Exchange。Conte com Nossa Equipe para o Projeto de Decoração de Seu Espaço. Peça Já Seu Orçamento。</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>https://vvv-kvcoln.site/ucenter/signin?bb83c1c0-bfde-4c3f-a832-2228d3afe621de56f320-d570-4766-a84d-57e73836f17c</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update 20220309 report pre check if there has any log havent submitted
</commit_message>
<xml_diff>
--- a/data_saved/exact_country_log.xlsx
+++ b/data_saved/exact_country_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M366"/>
+  <dimension ref="A1:M387"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23353,7 +23353,1252 @@
           <t>https://direcionapanfletagem.blogspot.com/2022/03/direciona-panfletagem-distribuicao-de.html?m=1</t>
         </is>
       </c>
-      <c r="M366" t="inlineStr"/>
+      <c r="M366" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>366</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.18 Safari/537.36 Edg/96.0.1054.5</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G367" s="2" t="n">
+        <v>44629.38779825231</v>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwij9ZP-7bf2AhWRm8IKHZevD-UYABAAGgJ0bQ&amp;sig=AOD64_0UT53oc15Y9wvYieo39AQAJS2DlQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=XAAoYrn9BIPWmAWt1oaoCg&amp;iflsig=AHkkrS4AAAAAYigObCjpuXbsIb6mip0QLzfkpF1PvnOi&amp;ved=0ahUKEwi5m_T77bf2AhUDK6YKHS2rAaUQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYN8XaABwAHgBgAFuiAGkA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Crypto Trading App (CFD) - plus500.at</t>
+        </is>
+      </c>
+      <c r="K367" t="inlineStr">
+        <is>
+          <t>Plus500 is the Main Sponsor of Atletico de Madrid football club</t>
+        </is>
+      </c>
+      <c r="L367" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency%20exchange_ks%2Bkwd-298401903980_tid%2Bp_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIo_WT_u239gIVkZvCCh2Xrw_lEAAYASAAEgLoxPD_BwE</t>
+        </is>
+      </c>
+      <c r="M367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>367</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; moto g play (2021)) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/85.0.4183.127 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>kn-IN</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>kn-IN</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G368" s="2" t="n">
+        <v>44629.41077255787</v>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjChLCw9bf2AhXCqZYKHY5JCGEYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_0ZeMjP3gcgAdxyjDMwuMFnmHuVNw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=HAgoYsPMNLTFmAXknoCQBQ&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gKYNMXaABwAHgBgAFuiAGqA5IBAzAuNJgBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J368" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs on Bitcoin, Ethereum - plus500.at</t>
+        </is>
+      </c>
+      <c r="K368" t="inlineStr">
+        <is>
+          <t>Atletico Madrid &amp; Plus500</t>
+        </is>
+      </c>
+      <c r="L368" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIwoSwsPW39gIVwqmWCh2OSQhhEAAYASAAEgK2xPD_BwE</t>
+        </is>
+      </c>
+      <c r="M368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>368</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; zh-cn; BRQ-AN00 Build/HUAWEIBRQ-AN00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Chrome/77.0.3865.120 MQQBrowser/11.9 Mobile Safari/537.36 COVC/045717</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G369" s="2" t="n">
+        <v>44629.4241605787</v>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiDiojY-bf2AhVN2JYKHV0PD3kYABAAGgJ0bA&amp;sig=AOD64_1T3_IAZe3RdEJNk8nI0Bg5jN_wWg&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=oQwoYtnJM4_80gSTtY2QDA&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgNYNYXaABwAHgBgAFjiAHbApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J369" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Crypto Trading App (CFD) - plus500.at</t>
+        </is>
+      </c>
+      <c r="K369" t="inlineStr">
+        <is>
+          <t>Download now</t>
+        </is>
+      </c>
+      <c r="L369" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIg4qI2Pm39gIVTdiWCh1dDw95EAAYASAAEgI8bfD_BwE</t>
+        </is>
+      </c>
+      <c r="M369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>369</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/14.1.2 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G370" s="2" t="n">
+        <v>44629.4271146875</v>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiit-HR-rf2AhVxwRYFHfwEAXgYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_1f_CFqcS8pknwhQlxg9CE3-fjAgw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=oQ0oYp-gGauXr7wPjaq5wAs&amp;iflsig=AHkkrS4AAAAAYigbsYDGKAgClCEvirpSBS_0fE_aQhmt&amp;ved=0ahUKEwjf9PDP-rf2AhWry4sBHQ1VDrgQ4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgMYNUXaABwAHgBgAFziAGGA5IBAzMuMZgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J370" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Online Cryptocurrency Market - plus500.at</t>
+        </is>
+      </c>
+      <c r="K370" t="inlineStr">
+        <is>
+          <t>Trade with no surprises Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L370" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIorfh0fq39gIVccEWBR38BAF4EAAYASAAEgJuGfD_BwE</t>
+        </is>
+      </c>
+      <c r="M370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>370</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/99.0.4844.51 Safari/537.36 Edg/99.0.1150.30</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G371" s="2" t="n">
+        <v>44629.44862159722</v>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj5gN_Hgbj2AhV8wRYFHWUWDfcYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_3Q2POsUuCLcUU7u9SFMggRURDwdw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=4hQoYselKKSzmAW-hr_YDg&amp;iflsig=AHkkrS4AAAAAYigi8gzUzATbwMTWcEOitH4ygo-6G1_5&amp;ved=0ahUKEwjHnr7Fgbj2AhWkGaYKHT7DD-sQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgJYNMXaABwAHgBgAFxiAGqA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J371" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs on Bitcoin, Ethereum - plus500.at</t>
+        </is>
+      </c>
+      <c r="K371" t="inlineStr">
+        <is>
+          <t>Trade with no surprises Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L371" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI-YDfx4G49gIVfMEWBR1lFg33EAAYASAAEgKMhvD_BwE</t>
+        </is>
+      </c>
+      <c r="M371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>371</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; en-us; Infinix X657 Build/QP1A.190711.020) AppleWebKit/533.1 (KHTML, like Gecko) Mobile Safari/533.1</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G372" s="2" t="n">
+        <v>44629.49105560185</v>
+      </c>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj2342cj7j2AhVJq5YKHUVCAtgYABAAGgJ0bA&amp;sig=AOD64_1MKkl9F41gu4dw-5Di5NKbVxHxyQ&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=NSMoYvurO9yGr7wPqqC0-As&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNYXaABwAHgCgAFbiAHjApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J372" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs on Bitcoin, Ethereum - plus500.at</t>
+        </is>
+      </c>
+      <c r="K372" t="inlineStr">
+        <is>
+          <t>Download now</t>
+        </is>
+      </c>
+      <c r="L372" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI9t-NnI-49gIVSauWCh1FQgLYEAAYASAAEgLhO_D_BwE</t>
+        </is>
+      </c>
+      <c r="M372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>372</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.93 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G373" s="2" t="n">
+        <v>44629.49157516204</v>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjFpMqxj7j2AhXSwRYFHUD1DycYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_03lMoSrqi9NAULVLsEN4U4DTDW2w&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=YyMoYvSMA8CKr7wPwcaj4AI&amp;iflsig=AHkkrS4AAAAAYigxc6sAarMf1ukC2Ig-gau74X35h-uR&amp;ved=0ahUKEwi0ytivj7j2AhVAxYsBHUHjCCwQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNUXaABwAHgBgAGlAogBzQSSAQUxLjIuMZgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J373" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs: Bitcoin, Ethereum &amp; More - plus500.at</t>
+        </is>
+      </c>
+      <c r="K373" t="inlineStr">
+        <is>
+          <t>Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L373" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIxaTKsY-49gIV0sEWBR1A9Q8nEAAYASAAEgI5cvD_BwE</t>
+        </is>
+      </c>
+      <c r="M373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>373</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10.14; rv:97.0) Gecko/20100101 Firefox/97.0</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>mr-IN</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>mr-IN</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G374" s="2" t="n">
+        <v>44629.4938928125</v>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj7iICRkLj2AhVKqpYKHUXXD-sYABAAGgJ0bA&amp;sig=AOD64_0NTwYGqZst_Wm6uQri2UVjHny0ow&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=KyQoYoDEDPTomAWcgoPoDQ&amp;iflsig=AHkkrS4AAAAAYigyOzdDTwJFNQme6rU10KCW5qk9qP3C&amp;ved=0ahUKEwjAhZGPkLj2AhV0NKYKHRzBAN0Q4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNUXaABwAHgBgAFqiAGHA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J374" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Online Cryptocurrency Market - plus500.at</t>
+        </is>
+      </c>
+      <c r="K374" t="inlineStr">
+        <is>
+          <t>Plus500 is the Main Sponsor of Atletico de Madrid football club</t>
+        </is>
+      </c>
+      <c r="L374" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI-4iAkZC49gIVSqqWCh1F1w_rEAAYASAAEgIgqfD_BwE</t>
+        </is>
+      </c>
+      <c r="M374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>374</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; BLA-AL00 Build/HUAWEIBLA-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G375" s="2" t="n">
+        <v>44629.49491910879</v>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjXt6y7kLj2AhWGTmAKHUMbBrsYABAAGgJ0bQ&amp;sig=AOD64_20FPOufKBPG5HAaTNpc7Xbr1TuqQ&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=gyQoYpLmOYeWr7wP5LiE-A4&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNAXaABwAHgBgAFviAGIA5IBAzMuMZgBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J375" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Free Demo, 0 Commissions</t>
+        </is>
+      </c>
+      <c r="K375" t="inlineStr">
+        <is>
+          <t>Capital at risk. Bitcoin CFD Trading. Try our Free Demo and check the Market Movements!</t>
+        </is>
+      </c>
+      <c r="L375" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI17esu5C49gIVhk5gCh1DGwa7EAAYASAAEgILBPD_BwE</t>
+        </is>
+      </c>
+      <c r="M375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>375</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; en-us; Infinix X657 Build/QP1A.190711.020) AppleWebKit/533.1 (KHTML, like Gecko) Mobile Safari/533.1</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G376" s="2" t="n">
+        <v>44629.52049040509</v>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiQ0ujYmLj2AhXRq5YKHXikDqIYABAAGgJ0bA&amp;sig=AOD64_34ShoAY9450GW54EHNkpDSxG3PfA&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=JS0oYvTKDauEr7wPwOagEA&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgMYNIXaABwAHgBgAFqiAGUA5IBAzEuM5gBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J376" t="inlineStr">
+        <is>
+          <t>Online Cryptocurrency Market - 2022 Bitcoin CFDs</t>
+        </is>
+      </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>Google Play</t>
+        </is>
+      </c>
+      <c r="L376" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIkNLo2Ji49gIV0auWCh14pA6iEAAYASAAEgKVsfD_BwE</t>
+        </is>
+      </c>
+      <c r="M376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>376</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/98.0.4758.102 Safari/537.36 Edg/98.0.1108.62</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G377" s="2" t="n">
+        <v>44629.52106440972</v>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj8hLbwmLj2AhWKdmAKHQTlCk0YABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1Ugldv7NVtBfqutrlTB2SW27nWGw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=Vi0oYvmDCsmGr7wPiZKpwAg&amp;iflsig=AHkkrS4AAAAAYig7Zr5pG9YW6OIXw94k9sFuffa2z3KP&amp;ved=0ahUKEwj5hqDumLj2AhVJw4sBHQlJCogQ4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgIYOUXaABwAHgAgAFjiAHqApIBATSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J377" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Buy &amp; Sell Cryptocurrency CFDs - plus500.at</t>
+        </is>
+      </c>
+      <c r="K377" t="inlineStr">
+        <is>
+          <t>Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L377" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI_IS28Ji49gIVinZgCh0E5QpNEAAYASAAEgKQKfD_BwE</t>
+        </is>
+      </c>
+      <c r="M377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>377</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; ALP-AL00 Build/HUAWEIALP-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G378" s="2" t="n">
+        <v>44629.75734324074</v>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwimvPP25Lj2AhXIUGAKHb26BzQYABAAGgJ0bQ&amp;sig=AOD64_1J7DoUMLLVm7qupSWayvxuY2hRJA&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=FX0oYoTcGNTEmAXZgb_YBg&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gMYOUXaABwAHgBgAFfiAHqApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J378" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs: Bitcoin, Ethereum &amp; More</t>
+        </is>
+      </c>
+      <c r="K378" t="inlineStr">
+        <is>
+          <t>Capital at risk. Bitcoin CFD Trading. Try our Free Demo and check the Market Movements! Trade CFD with a Regulated Broker, 0 Commissions&amp;Tight Spreads. Award winning CFD-Platform。</t>
+        </is>
+      </c>
+      <c r="L378" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency%20exchange_ks%2Bkwd-298401903980_tid%2Bp_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIprzz9uS49gIVyFBgCh29ugc0EAAYASAAEgIyZfD_BwE</t>
+        </is>
+      </c>
+      <c r="M378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>378</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/15.3 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G379" s="2" t="n">
+        <v>44629.75876077546</v>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjv8Pew5bj2AhWbvZYKHat-CNcYABAAGgJ0bA&amp;ae=2&amp;sig=AOD64_2BFGrE4GlgCIudFNQqiv_vqyI96Q&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=j30oYqGHCbmVr7wP_syswAc&amp;iflsig=AHkkrS4AAAAAYiiLnxkZRiSYoFwoM5qLaOqaRAcuYyXd&amp;ved=0ahUKEwjhioav5bj2AhW5yosBHX4mC3gQ4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYM8XaABwAHgDgAFkiAH4ApIBAzMuMZgBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J379" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Seize the Market Volatility - plus500.at</t>
+        </is>
+      </c>
+      <c r="K379" t="inlineStr">
+        <is>
+          <t>Atletico de Madrid football club</t>
+        </is>
+      </c>
+      <c r="L379" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI7_D3sOW49gIVm72WCh2rfgjXEAAYASAAEgKK7fD_BwE</t>
+        </is>
+      </c>
+      <c r="M379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>379</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/99.0.4844.51 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G380" s="2" t="n">
+        <v>44629.76497121528</v>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiArfqw57j2AhVLdmAKHVB_ABwYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_2Rfk0sFSbmDtYxEuja4CkBMxk0hA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=pn8oYsynF_CsmAW8j5HoCQ&amp;iflsig=AHkkrS4AAAAAYiiNto97UhIRNJUQ4O9MwnnSd3B8smoN&amp;ved=0ahUKEwjMkqKu57j2AhVwFqYKHbxHBJ0Q4dUDCAc&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgIYM0XaABwAHgBgAFwiAGdA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J380" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Buy &amp; Sell Cryptocurrency CFDs - plus500.at</t>
+        </is>
+      </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L380" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIgK36sOe49gIVS3ZgCh1QfwAcEAAYASAAEgIBa_D_BwE</t>
+        </is>
+      </c>
+      <c r="M380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>380</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10.15; rv:97.0) Gecko/20100101 Firefox/97.0</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>hi-IN</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>hi-IN</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G381" s="2" t="n">
+        <v>44629.78692680556</v>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwik1aq57rj2AhXLuZYKHYgNB0gYABAAGgJ0bA&amp;sig=AOD64_30DxOCjikXCjnaDcAFk29raFPsrw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=EIcoYvrMC52Ir7wPxc65uAc&amp;iflsig=AHkkrS4AAAAAYiiVINL3JoojA-8Mbfk5-CnprM3i8rs-&amp;ved=0ahUKEwj6lJu37rj2AhUdxIsBHUVnDncQ4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNAXaABwAHgBgAGYAYgBqgSSAQMwLjSYAQCgAQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J381" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Bitcoin CFD Trading - plus500.at</t>
+        </is>
+      </c>
+      <c r="K381" t="inlineStr">
+        <is>
+          <t>Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L381" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIpNWque649gIVy7mWCh2IDQdIEAAYASAAEgLl7vD_BwE</t>
+        </is>
+      </c>
+      <c r="M381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>381</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; HRY-AL00a Build/HONORHRY-AL00a) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G382" s="2" t="n">
+        <v>44629.79247497685</v>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjF55ie8Lj2AhXMqJYKHfg5Bz4YABAAGgJ0bA&amp;sig=AOD64_0g8JU8rY-B60n95jHFklnvo59B6Q&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=8IgoYu2cIcyZr7wP-bqK0Ak&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgKYNEXaABwAHgCgAFXiAHSApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>Crypto Trading App (CFD) - 2022 Bitcoin CFDs - plus500.at</t>
+        </is>
+      </c>
+      <c r="K382" t="inlineStr">
+        <is>
+          <t>Download now</t>
+        </is>
+      </c>
+      <c r="L382" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIxeeYnvC49gIVzKiWCh34OQc-EAAYASAAEgKJGvD_BwE</t>
+        </is>
+      </c>
+      <c r="M382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>382</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 10; en-us; Infinix X657 Build/QP1A.190711.020) AppleWebKit/533.1 (KHTML, like Gecko) Mobile Safari/533.1</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G383" s="2" t="n">
+        <v>44629.79489329861</v>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiFydGB8bj2AhWNQ2AKHbQPCbQYABAAGgJ0bQ&amp;sig=AOD64_1CRo49D3RtI4VcD_6e-RC-EIh_yg&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=wYkoYsXgA7CwmAWFtZnYAw&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gKYNUXaABwAHgDgAFoiAGWA5IBAzEuM5gBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - CFDs on Bitcoin, Ethereum - plus500.at</t>
+        </is>
+      </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>Download now</t>
+        </is>
+      </c>
+      <c r="L383" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIhcnRgfG49gIVjUNgCh20Dwm0EAAYASAAEgKACfD_BwE</t>
+        </is>
+      </c>
+      <c r="M383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>383</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; EML-AL00 Build/HUAWEIEML-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G384" s="2" t="n">
+        <v>44629.80701236111</v>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSyJH19Lj2AhVLsZYKHbAZDeEYABAAGgJ0bA&amp;sig=AOD64_2yqtxhAfj7NPV0WwDb63NVURKLBA&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=2I0oYrnfIZuJr7wPquWP4Ag&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gKYPIXaABwAHgDgAFtiAHzApIBAzMuMZgBAKABAbABAA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J384" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Crypto Trading App (CFD) - plus500.at</t>
+        </is>
+      </c>
+      <c r="K384" t="inlineStr">
+        <is>
+          <t>Google Play</t>
+        </is>
+      </c>
+      <c r="L384" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIksiR9fS49gIVS7GWCh2wGQ3hEAAYASAAEgLlY_D_BwE</t>
+        </is>
+      </c>
+      <c r="M384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>384</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; rv:91.0) Gecko/20100101 Firefox/91.0</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>mr-IN</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>mr-IN</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G385" s="2" t="n">
+        <v>44629.80754229167</v>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi40vaK9bj2AhUF10wCHS8xC-MYABAAGgJ0bQ&amp;sig=AOD64_0zeR6RV_eXpHwMPd_wF2_8NYucvA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=Bo4oYo7FEqOwmAW6yrXAAw&amp;iflsig=AHkkrS4AAAAAYiicFnkftOoSe29rHYkppfcLvBYJQcJy&amp;ved=0ahUKEwiO4P6I9bj2AhUjGKYKHTplDTgQ4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgMYPUXaABwAHgBgAFziAGoA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J385" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Buy &amp; Sell Cryptocurrency CFDs</t>
+        </is>
+      </c>
+      <c r="K385" t="inlineStr">
+        <is>
+          <t>Trade with no surprises Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L385" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIuNL2ivW49gIVBddMAh0vMQvjEAAYASAAEgIO-vD_BwE</t>
+        </is>
+      </c>
+      <c r="M385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>385</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:96.0) Gecko/20100101 Firefox/96.0</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>tr-TR</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G386" s="2" t="n">
+        <v>44629.81344230324</v>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwijl9n99rj2AhVJVGAKHbGxBBgYABAAGgJ0bQ&amp;sig=AOD64_3yx7HYnRieS-htAFU3VllN9YIOSA&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=A5AoYvD-F5iJr7wP7YOEkA4&amp;iflsig=AHkkrS4AAAAAYiieExfr6qITyt5hTYWan1KqSde7owXn&amp;ved=0ahUKEwiwjN_79rj2AhWYxIsBHe0BAeIQ4dUDCAY&amp;uact=5&amp;oq=kucoin+exchange&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBAgAEB5QAFgKYNEXaABwAHgBgAFyiAGkA5IBAzEuM5gBAKABAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+      <c r="J386" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Buy and Sell Bitcoin CFDs - plus500.at</t>
+        </is>
+      </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>Trade with no surprises Check out our transparent fees</t>
+        </is>
+      </c>
+      <c r="L386" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226778_agi%2BCrypto.Bitcoins_English.AT_agn%2Bbitcoins_ks%2Bkwd-20856201099_tid%2Bb_mt%2Bc_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIo5fZ_fa49gIVSVRgCh2xsQQYEAAYASAAEgJoVfD_BwE</t>
+        </is>
+      </c>
+      <c r="M386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; HRY-AL00a Build/HONORHRY-AL00a) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G387" s="2" t="n">
+        <v>44629.83322072231</v>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjl3fms_bj2AhVBeYsKHdwYA4MYABAAGgJ0bQ&amp;sig=AOD64_0IzEGSYvn7VGwOV-ceLMPzj2KXsQ&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=sZYoYp7JCaremAWEmKWoCA&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBlgTYOgXaABwAHgBgAFjiAH2ApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J387" t="inlineStr">
+        <is>
+          <t>CFD 買賣 平台 - CFD 網 上 交易 平台 - CFD 平台交易</t>
+        </is>
+      </c>
+      <c r="K387" t="inlineStr">
+        <is>
+          <t>Google Play</t>
+        </is>
+      </c>
+      <c r="L387" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11444535488_cpi%2BWorldChinese1SearchPartners-1408_cp%2B137328966841_agi%2BTrading.Trading_English.AT_agn%2Btrading_ks%2Bkwd-10427121_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMI5d35rP249gIVQXmLCh3cGAODEAAYASAAEgLhtPD_BwE</t>
+        </is>
+      </c>
+      <c r="M387" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update 20220309 report pre check if there has any log havent submitted -exact country scarpper
</commit_message>
<xml_diff>
--- a/data_saved/exact_country_log.xlsx
+++ b/data_saved/exact_country_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M387"/>
+  <dimension ref="A1:M391"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24540,10 +24540,8 @@
       <c r="M386" t="inlineStr"/>
     </row>
     <row r="387">
-      <c r="A387" t="inlineStr">
-        <is>
-          <t>386</t>
-        </is>
+      <c r="A387" t="n">
+        <v>386</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
@@ -24571,7 +24569,7 @@
         </is>
       </c>
       <c r="G387" s="2" t="n">
-        <v>44629.83322072231</v>
+        <v>44629.83322071759</v>
       </c>
       <c r="H387" t="inlineStr">
         <is>
@@ -24599,6 +24597,244 @@
         </is>
       </c>
       <c r="M387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>387</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; U; Android 8.2.0; ko-kr; SHW-M440S Build/JZO54K) AppleWebKit/534.30 (KHTML, like Gecko) Version/4.0 Mobile Safari/534.30 NAVER(inapp; search; 250; 5.2.0)</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>de-DE</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G388" s="2" t="n">
+        <v>44629.85711163194</v>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiXxIeFhbn2AhXU0ZYKHSc4DMMYABAAGgJ0bA&amp;sig=AOD64_1qbjc4M15H1OawdNH0HEMgHe90Lw&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=wJ4oYvm9LZiKr7wP0pi36AU&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gLYN4XaABwAHgAgAFgiAH3ApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J388" t="inlineStr">
+        <is>
+          <t>CFD 平台交易 - CFD 交易平台</t>
+        </is>
+      </c>
+      <c r="K388" t="inlineStr">
+        <is>
+          <t>Google Play</t>
+        </is>
+      </c>
+      <c r="L388" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11444535488_cpi%2BWorldChinese1SearchPartners-1408_cp%2B137328966841_agi%2BTrading.Trading_English.AT_agn%2Btrading_ks%2Bkwd-10427121_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIl8SHhYW59gIV1NGWCh0nOAzDEAAYASAAEgIAM_D_BwE</t>
+        </is>
+      </c>
+      <c r="M388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>388</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 14_7_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) FxiOS/36.0  Mobile/15E148 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>pt-BR</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G389" s="2" t="n">
+        <v>44629.86273104166</v>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiCocjshrn2AhUk3EwCHfKbBiwYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_1Vy7SeKv4OcRCWx7U4l62cspqCJw&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=pqAoYu33G4rl0ASl87eoBg&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgMYN8XaABwAHgCgAFdiAHtApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t>2022 Bitcoin CFDs - Trading Bitcoin CFDs - Crypto CFDs - plus500.at</t>
+        </is>
+      </c>
+      <c r="K389" t="inlineStr">
+        <is>
+          <t>Real Time Index Rates</t>
+        </is>
+      </c>
+      <c r="L389" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226778_agi%2BCrypto.Bitcoins_English.AT_agn%2Bbitcoine_ks%2Bkwd-298782581900_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gbraid=0AAAAAD2rQn8od-FIr81uT3c5LZl60JB4A&amp;gclid=EAIaIQobChMIgqHI7Ia59gIVJNxMAh3ymwYsEAAYASAAEgLnIfD_BwE</t>
+        </is>
+      </c>
+      <c r="M389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>389</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 12_0 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) FxiOS/13.2b11866 Mobile/16A366 Safari/605.1.15</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>nl-NL</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G390" s="2" t="n">
+        <v>44629.87846986111</v>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiooun0i7n2AhUXWmAKHaeTDdYYABAAGgJ0bQ&amp;ae=2&amp;sig=AOD64_3yt-zV3isfxd-ehTHuND5uvt4yMQ&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=9aUoYqmbJcaUr7wP4rqX6Ao&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQA1gMYN8XaABwAHgBgAFbiAHaApIBATSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>CFD 平台交易 - cfd 平台 - CFD 買賣 平台 - plus500.at</t>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t>资本有风险. 关于加密数字货币、外汇、股票、商品、期权、ETF和指数的CFD。查看我们的实时财经日历. 获取实时市场通知。2000+ Instruments。</t>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11444535488_cpi%2BWorldChinese1SearchPartners-1408_cp%2B137328966841_agi%2BTrading.Trading_English.AT_agn%2Btrading_ks%2Bkwd-10427121_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMIqKLp9Iu59gIVF1pgCh2nkw3WEAAYASAAEgLdPfD_BwE</t>
+        </is>
+      </c>
+      <c r="M390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>390</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>kucoin exchange</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; ALP-AL00 Build/HUAWEIALP-AL00) AppleWebKit/537.36 (KHTML, like Gecko) Version/4.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>hi-IN</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>hi-IN</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>desktop</t>
+        </is>
+      </c>
+      <c r="G391" s="2" t="n">
+        <v>44629.89703810363</v>
+      </c>
+      <c r="H391" t="inlineStr">
+        <is>
+          <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiZ3uPxkbn2AhXRwpYKHZqGAK4YABAAGgJ0bA&amp;sig=AOD64_2v_AFgSYTZ0clJsrwV8Dm9mi2WdQ&amp;rct=j&amp;q&amp;adurl</t>
+        </is>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=kucoin+exchange&amp;source=hp&amp;ei=OawoYoePOoKJmAXFkK-gAg&amp;oq=kucoin+exchange&amp;gs_lcp=ChFtb2JpbGUtZ3dzLXdpei1ocBADMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgAQyBQgAEIAEMgUIABCABDIFCAAQgARQBFgLYNkXaABwAHgCgAGEAYgBhASSAQMwLjSYAQCgAQGwAQA&amp;sclient=mobile-gws-wiz-hp</t>
+        </is>
+      </c>
+      <c r="J391" t="inlineStr">
+        <is>
+          <t>Plus500 CFD - Crypto Trading - Online Cryptocurrency Market</t>
+        </is>
+      </c>
+      <c r="K391" t="inlineStr">
+        <is>
+          <t>Download now</t>
+        </is>
+      </c>
+      <c r="L391" t="inlineStr">
+        <is>
+          <t>https://www.plus500.at/zh?id=1408&amp;tags=g_sr%2B11490222447_cpi%2BWorldChinese1SearchCrypto-1408_cp%2B135006226938_agi%2BCrypto.CryptoCurrency_English.AT_agn%2Bcryptocurrency_ks%2Bkwd-24551837799_tid%2Bb_mt%2Bm_de%2Bg_nt%2B_ext%2B2344_loc%2BUURL&amp;%D7%90&amp;gclid=EAIaIQobChMImd7j8ZG59gIV0cKWCh2ahgCuEAAYASAAEgKwBPD_BwE</t>
+        </is>
+      </c>
+      <c r="M391" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>